<commit_message>
Deploying to gh-pages from  @ 5b6c8c1fbc985111425ba3e945757648729aecd1 🚀
</commit_message>
<xml_diff>
--- a/2021-01-26.xlsx
+++ b/2021-01-26.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CDD96B-211D-404A-AFE2-E4C920CD37E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA910BE-56D5-4DA3-A461-DF6863CBA036}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="28512" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterung" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
   <si>
     <t>Bayern</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>Datenstand: 27.01.2021, 10:00 Uhr</t>
+  </si>
+  <si>
+    <t>Bayern*</t>
+  </si>
+  <si>
+    <t>* Enthält eine Korrektur der am 26.01.2021 veröffentlichten Daten für Bayern. Daher liegen die Werte heute niedriger als am 26.01.2021 berichtet.</t>
   </si>
 </sst>
 </file>
@@ -594,9 +600,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -683,7 +686,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -747,6 +749,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1160,111 +1166,111 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="148.44140625" style="9" customWidth="1"/>
-    <col min="2" max="16384" width="11.44140625" style="9"/>
+    <col min="1" max="1" width="148.42578125" style="9" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
         <v>59</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="41"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="45" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="44" t="s">
+    <row r="6" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="41"/>
-    </row>
-    <row r="10" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="45" t="s">
+    <row r="9" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="40"/>
+    </row>
+    <row r="10" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="40"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="51" t="s">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="50" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="40"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="41" t="s">
+    <row r="13" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="39"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="40" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="45" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="52" t="s">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="51" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="40"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="40"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="39"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="50" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="49" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="49" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="50" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="49" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1279,605 +1285,605 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="5" width="11.44140625" style="9"/>
-    <col min="7" max="7" width="12.33203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="5" width="11.42578125" style="9"/>
+    <col min="7" max="7" width="12.28515625" style="9" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="60" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="62"/>
-    </row>
-    <row r="2" spans="1:11" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="54" t="s">
+      <c r="J1" s="60"/>
+    </row>
+    <row r="2" spans="1:11" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="54"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="67" t="s">
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="65" t="s">
+      <c r="H2" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="63" t="s">
+      <c r="I2" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="65" t="s">
+      <c r="J2" s="63" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="57"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="27" t="s">
+    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="55"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="68"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="66"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G3" s="66"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="64"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="34">
         <v>228138</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <v>189426</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <v>186964</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>2462</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <v>7961</v>
       </c>
-      <c r="H4" s="34">
+      <c r="H4" s="33">
         <v>1.7064799681885165</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="29">
         <v>38712</v>
       </c>
-      <c r="J4" s="21">
+      <c r="J4" s="20">
         <v>5695</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="36">
+        <v>60</v>
+      </c>
+      <c r="C5" s="35">
         <v>365003</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <v>278653</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="21">
         <v>269556</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="21">
         <v>9097</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="22">
         <v>10696</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="23">
         <v>2.1231130193313588</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="30">
         <v>86350</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="24">
         <v>5143</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="34">
         <v>103639</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>81198</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <v>79264</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="16">
         <v>1934</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="17">
         <v>3138</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="18">
         <v>2.21278646002947</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="29">
         <v>22441</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="20">
         <v>2646</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="35">
         <v>68478</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <v>65723</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="21">
         <v>65723</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="21">
         <v>0</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="22">
         <v>2277</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="23">
         <v>2.6060978796483436</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="30">
         <v>2755</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="24">
         <v>1610</v>
       </c>
-      <c r="K7" s="42"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K7" s="41"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="34">
         <v>19825</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>17072</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <v>15814</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="16">
         <v>1258</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="17">
         <v>585</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="18">
         <v>2.5061582320662592</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="29">
         <v>2753</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="20">
         <v>631</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="35">
         <v>44231</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="21">
         <v>39140</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="21">
         <v>38830</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="21">
         <v>310</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="22">
         <v>1446</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="23">
         <v>2.1188218397804737</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="30">
         <v>5091</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="24">
         <v>601</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="34">
         <v>141478</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <v>108901</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="16">
         <v>108901</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="16">
         <v>0</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="17">
         <v>4613</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="18">
         <v>1.7318640984211395</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="29">
         <v>32577</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="20">
         <v>2932</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="36">
         <v>62212</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="21">
         <v>52331</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="21">
         <v>51001</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="21">
         <v>1330</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="22">
         <v>805</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="23">
         <v>3.2541361500070267</v>
       </c>
-      <c r="I11" s="31">
+      <c r="I11" s="30">
         <v>9881</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11" s="24">
         <v>3920</v>
       </c>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="34">
         <v>152734</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <v>137227</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="16">
         <v>135323</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="16">
         <v>1904</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="17">
         <v>1926</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="18">
         <v>1.7167091506113386</v>
       </c>
-      <c r="I12" s="30">
+      <c r="I12" s="29">
         <v>15507</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="20">
         <v>6495</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="36">
+      <c r="C13" s="35">
         <v>357370</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="21">
         <v>295738</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="21">
         <v>295738</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="21">
         <v>0</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="22">
         <v>2991</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="23">
         <v>1.6478205734469977</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="30">
         <v>61632</v>
       </c>
-      <c r="J13" s="25">
+      <c r="J13" s="24">
         <v>5154</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="34">
         <v>139626</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="16">
         <v>134587</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="16">
         <v>130782</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="16">
         <v>3805</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="17">
         <v>4736</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="18">
         <v>3.2874985069260316</v>
       </c>
-      <c r="I14" s="30">
+      <c r="I14" s="29">
         <v>5039</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="20">
         <v>637</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="36">
+      <c r="C15" s="35">
         <v>24255</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="21">
         <v>18835</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="21">
         <v>18347</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="21">
         <v>488</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="22">
         <v>763</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H15" s="23">
         <v>1.9085265081007248</v>
       </c>
-      <c r="I15" s="31">
+      <c r="I15" s="30">
         <v>5420</v>
       </c>
-      <c r="J15" s="25">
+      <c r="J15" s="24">
         <v>754</v>
       </c>
-      <c r="K15" s="42"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K15" s="41"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="34">
         <v>86187</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <v>77181</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="16">
         <v>76992</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="16">
         <v>189</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="17">
         <v>3458</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="18">
         <v>1.895421160907089</v>
       </c>
-      <c r="I16" s="30">
+      <c r="I16" s="29">
         <v>9006</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="20">
         <v>2643</v>
       </c>
-      <c r="K16" s="42"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K16" s="41"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="36">
+      <c r="C17" s="35">
         <v>59750</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="21">
         <v>45020</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="21">
         <v>44445</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="21">
         <v>575</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="22">
         <v>1225</v>
       </c>
-      <c r="H17" s="24">
+      <c r="H17" s="23">
         <v>2.0512287780745422</v>
       </c>
-      <c r="I17" s="31">
+      <c r="I17" s="30">
         <v>14730</v>
       </c>
-      <c r="J17" s="25">
+      <c r="J17" s="24">
         <v>1723</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="35">
+      <c r="C18" s="34">
         <v>91473</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="16">
         <v>87065</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="16">
         <v>86756</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="16">
         <v>309</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="17">
         <v>1430</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="18">
         <v>2.9983404350133429</v>
       </c>
-      <c r="I18" s="30">
+      <c r="I18" s="29">
         <v>4408</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="20">
         <v>1613</v>
       </c>
-      <c r="K18" s="42"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K18" s="41"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="36">
+      <c r="C19" s="35">
         <v>46490</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="21">
         <v>44118</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="21">
         <v>44118</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="21">
         <v>0</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="22">
         <v>2564</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H19" s="23">
         <v>2.0679879515022654</v>
       </c>
-      <c r="I19" s="31">
+      <c r="I19" s="30">
         <v>2372</v>
       </c>
-      <c r="J19" s="25">
+      <c r="J19" s="24">
         <v>330</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="38">
+      <c r="C20" s="37">
         <f>D20+I20</f>
         <v>1990889</v>
       </c>
@@ -1901,25 +1907,28 @@
         <f>D20/83166711*100</f>
         <v>2.0106782868929374</v>
       </c>
-      <c r="I20" s="29">
+      <c r="I20" s="28">
         <f>SUM(I4:I19)</f>
         <v>318674</v>
       </c>
-      <c r="J20" s="32">
+      <c r="J20" s="31">
         <f>SUM(J4:J19)</f>
         <v>42527</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="42" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="42" t="s">
+    <row r="22" spans="1:11" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="41" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
       <c r="D23" s="15"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C27" s="33"/>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1951,582 +1960,582 @@
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="9" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" style="9"/>
-    <col min="5" max="5" width="12.6640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="9" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="9"/>
+    <col min="5" max="5" width="12.7109375" style="9" customWidth="1"/>
     <col min="6" max="6" width="13" style="9" customWidth="1"/>
-    <col min="7" max="8" width="11.44140625" style="9"/>
-    <col min="9" max="9" width="13.33203125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="56.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.44140625" style="9"/>
+    <col min="7" max="8" width="11.42578125" style="9"/>
+    <col min="9" max="9" width="13.28515625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="56.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="71" t="s">
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-    </row>
-    <row r="2" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="27" t="s">
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+    </row>
+    <row r="2" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="72"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="19">
         <v>96829</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="17">
         <v>62226</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>6044</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="20">
         <v>37012</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="19">
         <v>17257</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="17">
         <v>13195</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="17">
         <v>673</v>
       </c>
-      <c r="J3" s="21">
+      <c r="J3" s="20">
         <v>7039</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="25">
         <v>100537</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="22">
         <v>143919</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <v>5612</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="24">
         <v>78081</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="25">
         <v>32478</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="22">
         <v>54743</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="22">
         <v>1086</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="24">
         <v>31692</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>58189</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>22786</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <v>108</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="20">
         <v>32102</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="19">
         <v>14859</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="17">
         <v>5685</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="17">
         <v>28</v>
       </c>
-      <c r="J5" s="21">
+      <c r="J5" s="20">
         <v>15872</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="25">
         <v>25325</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="22">
         <v>37633</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="22">
         <v>810</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="24">
         <v>13303</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="25">
         <v>21</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="22">
         <v>2734</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="22">
         <v>0</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="24">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="19">
         <v>3336</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <v>7319</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
         <v>129</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="20">
         <v>6253</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="19">
         <v>333</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="17">
         <v>957</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="17">
         <v>11</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="20">
         <v>1086</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="25">
         <v>15018</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="22">
         <v>18763</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="22">
         <v>1837</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="24">
         <v>10313</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="25">
         <v>1769</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="22">
         <v>2936</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="22">
         <v>34</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="24">
         <v>1946</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="19">
         <v>40228</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>52475</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <v>4731</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="20">
         <v>33975</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="19">
         <v>7783</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="17">
         <v>17194</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="17">
         <v>2806</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="20">
         <v>12533</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="25">
         <v>8722</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="22">
         <v>23520</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="22">
         <v>1093</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="24">
         <v>19778</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="25">
         <v>762</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="22">
         <v>5649</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="22">
         <v>84</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="24">
         <v>3520</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="19">
         <v>26246</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>75419</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="17">
         <v>21169</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="20">
         <v>59197</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="19">
         <v>3278</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="17">
         <v>7413</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="17">
         <v>3038</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="20">
         <v>7830</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="25">
         <v>0</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="22">
         <v>147967</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="22">
         <v>0</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="24">
         <v>147799</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="25">
         <v>0</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="22">
         <v>31390</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="22">
         <v>0</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="24">
         <v>31110</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="19">
         <v>51774</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="17">
         <v>51852</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="17">
         <v>77</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="20">
         <v>29224</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="19">
         <v>5</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="17">
         <v>2927</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="17">
         <v>7</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="20">
         <v>2100</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="25">
         <v>12775</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="22">
         <v>4698</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="22">
         <v>1</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="24">
         <v>5538</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="25">
         <v>4147</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="22">
         <v>611</v>
       </c>
-      <c r="I14" s="23">
+      <c r="I14" s="22">
         <v>0</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="24">
         <v>1995</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="19">
         <v>7892</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="17">
         <v>56037</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="17">
         <v>152</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="20">
         <v>20992</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="19">
         <v>701</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="17">
         <v>6989</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="17">
         <v>0</v>
       </c>
-      <c r="J15" s="21">
+      <c r="J15" s="20">
         <v>2017</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="25">
         <v>14741</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="22">
         <v>22640</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="22">
         <v>1926</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="24">
         <v>17018</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="25">
         <v>4784</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="22">
         <v>7538</v>
       </c>
-      <c r="I16" s="23">
+      <c r="I16" s="22">
         <v>947</v>
       </c>
-      <c r="J16" s="25">
+      <c r="J16" s="24">
         <v>6430</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="19">
         <v>25564</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="17">
         <v>26466</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="17">
         <v>5939</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="20">
         <v>21012</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="19">
         <v>1921</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="17">
         <v>713</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="17">
         <v>334</v>
       </c>
-      <c r="J17" s="21">
+      <c r="J17" s="20">
         <v>516</v>
       </c>
-      <c r="K17" s="42"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K17" s="41"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="22">
         <v>14989</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="22">
         <v>23187</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="22">
         <v>1790</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="24">
         <v>5700</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="22">
         <v>355</v>
       </c>
-      <c r="H18" s="23">
+      <c r="H18" s="22">
         <v>1748</v>
       </c>
-      <c r="I18" s="23">
+      <c r="I18" s="22">
         <v>4</v>
       </c>
-      <c r="J18" s="25">
+      <c r="J18" s="24">
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="3" t="s">
         <v>19</v>
@@ -2564,22 +2573,22 @@
         <v>125874</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C27" s="15"/>
     </row>
   </sheetData>
@@ -2602,19 +2611,19 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -2623,457 +2632,457 @@
       <c r="C1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="45" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="49">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="48">
         <v>44192</v>
       </c>
-      <c r="B2" s="43">
+      <c r="B2" s="42">
         <v>24268</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="46">
         <v>0</v>
       </c>
-      <c r="D2" s="47">
+      <c r="D2" s="46">
         <v>24268</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="49">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="48">
         <v>44193</v>
       </c>
-      <c r="B3" s="43">
+      <c r="B3" s="42">
         <v>19836</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="46">
         <v>0</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="46">
         <v>19836</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="49">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="48">
         <v>44194</v>
       </c>
-      <c r="B4" s="43">
+      <c r="B4" s="42">
         <v>43374</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="46">
         <v>0</v>
       </c>
-      <c r="D4" s="47">
+      <c r="D4" s="46">
         <v>43374</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="49">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="48">
         <v>44195</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="42">
         <v>57939</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="46">
         <v>0</v>
       </c>
-      <c r="D5" s="47">
+      <c r="D5" s="46">
         <v>57939</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="49">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="48">
         <v>44196</v>
       </c>
-      <c r="B6" s="43">
+      <c r="B6" s="42">
         <v>38510</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="46">
         <v>0</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="46">
         <v>38510</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="49">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="48">
         <v>44197</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="42">
         <v>24438</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="46">
         <v>0</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="46">
         <v>24438</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="49">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="48">
         <v>44198</v>
       </c>
-      <c r="B8" s="43">
+      <c r="B8" s="42">
         <v>51214</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="46">
         <v>0</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="46">
         <v>51214</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="49">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="48">
         <v>44199</v>
       </c>
-      <c r="B9" s="43">
+      <c r="B9" s="42">
         <v>24840</v>
       </c>
-      <c r="C9" s="47">
+      <c r="C9" s="46">
         <v>0</v>
       </c>
-      <c r="D9" s="47">
+      <c r="D9" s="46">
         <v>24840</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="49">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="48">
         <v>44200</v>
       </c>
-      <c r="B10" s="43">
+      <c r="B10" s="42">
         <v>48712</v>
       </c>
-      <c r="C10" s="47">
+      <c r="C10" s="46">
         <v>0</v>
       </c>
-      <c r="D10" s="47">
+      <c r="D10" s="46">
         <v>48712</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="49">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="48">
         <v>44201</v>
       </c>
-      <c r="B11" s="43">
+      <c r="B11" s="42">
         <v>51137</v>
       </c>
-      <c r="C11" s="47">
+      <c r="C11" s="46">
         <v>0</v>
       </c>
-      <c r="D11" s="47">
+      <c r="D11" s="46">
         <v>51137</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="49">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="48">
         <v>44202</v>
       </c>
-      <c r="B12" s="43">
+      <c r="B12" s="42">
         <v>56263</v>
       </c>
-      <c r="C12" s="47">
+      <c r="C12" s="46">
         <v>0</v>
       </c>
-      <c r="D12" s="47">
+      <c r="D12" s="46">
         <v>56263</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="49">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="48">
         <v>44203</v>
       </c>
-      <c r="B13" s="43">
+      <c r="B13" s="42">
         <v>58002</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="46">
         <v>0</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="46">
         <v>58002</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="49">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="48">
         <v>44204</v>
       </c>
-      <c r="B14" s="43">
+      <c r="B14" s="42">
         <v>58138</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C14" s="46">
         <v>0</v>
       </c>
-      <c r="D14" s="47">
+      <c r="D14" s="46">
         <v>58138</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="49">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="48">
         <v>44205</v>
       </c>
-      <c r="B15" s="43">
+      <c r="B15" s="42">
         <v>54252</v>
       </c>
-      <c r="C15" s="47">
+      <c r="C15" s="46">
         <v>0</v>
       </c>
-      <c r="D15" s="47">
+      <c r="D15" s="46">
         <v>54252</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="49">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="48">
         <v>44206</v>
       </c>
-      <c r="B16" s="43">
+      <c r="B16" s="42">
         <v>32466</v>
       </c>
-      <c r="C16" s="47">
+      <c r="C16" s="46">
         <v>0</v>
       </c>
-      <c r="D16" s="47">
+      <c r="D16" s="46">
         <v>32466</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="49">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="48">
         <v>44207</v>
       </c>
-      <c r="B17" s="43">
+      <c r="B17" s="42">
         <v>65731</v>
       </c>
-      <c r="C17" s="47">
+      <c r="C17" s="46">
         <v>0</v>
       </c>
-      <c r="D17" s="47">
+      <c r="D17" s="46">
         <v>65731</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="49">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="48">
         <v>44208</v>
       </c>
-      <c r="B18" s="43">
+      <c r="B18" s="42">
         <v>80238</v>
       </c>
-      <c r="C18" s="47">
+      <c r="C18" s="46">
         <v>0</v>
       </c>
-      <c r="D18" s="47">
+      <c r="D18" s="46">
         <v>80238</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="49">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="48">
         <v>44209</v>
       </c>
-      <c r="B19" s="43">
+      <c r="B19" s="42">
         <v>94189</v>
       </c>
-      <c r="C19" s="47">
+      <c r="C19" s="46">
         <v>0</v>
       </c>
-      <c r="D19" s="47">
+      <c r="D19" s="46">
         <v>94189</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="49">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="48">
         <v>44210</v>
       </c>
-      <c r="B20" s="43">
+      <c r="B20" s="42">
         <v>99981</v>
       </c>
-      <c r="C20" s="47">
+      <c r="C20" s="46">
         <v>0</v>
       </c>
-      <c r="D20" s="47">
+      <c r="D20" s="46">
         <v>99981</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="49">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="48">
         <v>44211</v>
       </c>
-      <c r="B21" s="43">
+      <c r="B21" s="42">
         <v>90731</v>
       </c>
-      <c r="C21" s="47">
+      <c r="C21" s="46">
         <v>225</v>
       </c>
-      <c r="D21" s="47">
+      <c r="D21" s="46">
         <v>90956</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="49">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="48">
         <v>44212</v>
       </c>
-      <c r="B22" s="43">
+      <c r="B22" s="42">
         <v>54427</v>
       </c>
-      <c r="C22" s="47">
+      <c r="C22" s="46">
         <v>466</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D22" s="46">
         <v>54893</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="49">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="48">
         <v>44213</v>
       </c>
-      <c r="B23" s="43">
+      <c r="B23" s="42">
         <v>30563</v>
       </c>
-      <c r="C23" s="47">
+      <c r="C23" s="46">
         <v>14301</v>
       </c>
-      <c r="D23" s="47">
+      <c r="D23" s="46">
         <v>44864</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="49">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="48">
         <v>44214</v>
       </c>
-      <c r="B24" s="43">
+      <c r="B24" s="42">
         <v>52070</v>
       </c>
-      <c r="C24" s="47">
+      <c r="C24" s="46">
         <v>16261</v>
       </c>
-      <c r="D24" s="47">
+      <c r="D24" s="46">
         <v>68331</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="49">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="48">
         <v>44215</v>
       </c>
-      <c r="B25" s="43">
+      <c r="B25" s="42">
         <v>57141</v>
       </c>
-      <c r="C25" s="47">
+      <c r="C25" s="46">
         <v>27427</v>
       </c>
-      <c r="D25" s="47">
+      <c r="D25" s="46">
         <v>84568</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="49">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="48">
         <v>44216</v>
       </c>
-      <c r="B26" s="43">
+      <c r="B26" s="42">
         <v>71945</v>
       </c>
-      <c r="C26" s="47">
+      <c r="C26" s="46">
         <v>47103</v>
       </c>
-      <c r="D26" s="47">
+      <c r="D26" s="46">
         <v>119048</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="49">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="48">
         <v>44217</v>
       </c>
-      <c r="B27" s="43">
+      <c r="B27" s="42">
         <v>57994</v>
       </c>
-      <c r="C27" s="47">
+      <c r="C27" s="46">
         <v>33834</v>
       </c>
-      <c r="D27" s="47">
+      <c r="D27" s="46">
         <v>91828</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="49">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="48">
         <v>44218</v>
       </c>
-      <c r="B28" s="43">
+      <c r="B28" s="42">
         <v>82083</v>
       </c>
-      <c r="C28" s="47">
+      <c r="C28" s="46">
         <v>30226</v>
       </c>
-      <c r="D28" s="47">
+      <c r="D28" s="46">
         <v>112309</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="49">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="48">
         <v>44219</v>
       </c>
-      <c r="B29" s="43">
+      <c r="B29" s="42">
         <v>47244</v>
       </c>
-      <c r="C29" s="47">
+      <c r="C29" s="46">
         <v>40557</v>
       </c>
-      <c r="D29" s="47">
+      <c r="D29" s="46">
         <v>87801</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="49">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="48">
         <v>44220</v>
       </c>
-      <c r="B30" s="43">
+      <c r="B30" s="42">
         <v>37243</v>
       </c>
-      <c r="C30" s="47">
+      <c r="C30" s="46">
         <v>28151</v>
       </c>
-      <c r="D30" s="47">
+      <c r="D30" s="46">
         <v>65394</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="49">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="48">
         <v>44221</v>
       </c>
-      <c r="B31" s="53">
+      <c r="B31" s="46">
         <v>56632</v>
       </c>
-      <c r="C31" s="53">
+      <c r="C31" s="46">
         <v>37596</v>
       </c>
-      <c r="D31" s="53">
+      <c r="D31" s="46">
         <v>94228</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="49">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="48">
         <v>44222</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="46">
         <v>50614</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="46">
         <v>42527</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="46">
         <v>93141</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="16" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="15">
+      <c r="B39" s="74">
         <f>SUM(B2:B35)</f>
         <v>1672215</v>
       </c>
-      <c r="C39" s="15">
+      <c r="C39" s="74">
         <f t="shared" ref="C39:D39" si="0">SUM(C2:C35)</f>
         <v>318674</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="74">
         <f t="shared" si="0"/>
         <v>1990889</v>
       </c>

</xml_diff>